<commit_message>
added low voltage check
</commit_message>
<xml_diff>
--- a/docs/comm_protocol_values.xlsx
+++ b/docs/comm_protocol_values.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>Information</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Length of Packet (# of Tags)</t>
+  </si>
+  <si>
+    <t>Low Voltage</t>
+  </si>
+  <si>
+    <t>0xF0</t>
   </si>
 </sst>
 </file>
@@ -590,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1000,6 +1006,14 @@
       <c r="H25" s="4"/>
       <c r="I25" s="8" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="G26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>